<commit_message>
fixed compute tax bug
</commit_message>
<xml_diff>
--- a/backend/tax_table.xlsx
+++ b/backend/tax_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahluw/PycharmProjects/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahluw/PycharmProjects/cpAI_EECS_498/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FD36C4-E5B1-DC4C-ACD2-2E65A43644C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F3CDA4-2823-6142-BF4D-7CF72337625F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15340" xr2:uid="{25D31A53-D8D8-9742-BA46-D6171DC6B6AC}"/>
   </bookViews>
@@ -47,10 +47,10 @@
     <t>married filing jointly</t>
   </si>
   <si>
-    <t>married filing          separately</t>
+    <t>head of household</t>
   </si>
   <si>
-    <t>head of household</t>
+    <t>married filing separately</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:F2063"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,10 +457,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>